<commit_message>
Fixed Telegram module import issue, added software management functions, and updated software expiry dates
</commit_message>
<xml_diff>
--- a/software_expiry_dates.xlsx
+++ b/software_expiry_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galiev_d\PycharmProjects\calendar_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFEB4C8-6C91-407E-B2B0-B268B5927EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5AAFA8-D287-4DF7-B88C-CCCC298ED52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="32175" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="1995" windowWidth="32145" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Имя продукта</t>
   </si>
@@ -28,40 +28,157 @@
     <t>Дата окончания</t>
   </si>
   <si>
-    <t>nanoCAD 24.0</t>
-  </si>
-  <si>
-    <t>nanoCAD Металлоконструкции 22.0</t>
-  </si>
-  <si>
-    <t>nanoCAD Металлоконструкции 23.0</t>
-  </si>
-  <si>
-    <t>nanoCAD BIM Вентиляция 23.1</t>
-  </si>
-  <si>
-    <t>nanoCAD BIM Электро 23.0</t>
-  </si>
-  <si>
-    <t>nanoCAD BIM Отопление 23.0</t>
-  </si>
-  <si>
-    <t>nanoCAD BIM Отопление 24.0</t>
-  </si>
-  <si>
     <t>АРГО</t>
   </si>
   <si>
     <t>Адепт:Смета</t>
   </si>
   <si>
-    <t>nanoCAD 23.0</t>
-  </si>
-  <si>
-    <t>nanoCAD BIM Вентиляция 22.0</t>
-  </si>
-  <si>
-    <t>nanoCAD BIM Электро 24.0</t>
+    <t>УЗ Селдон 1.7</t>
+  </si>
+  <si>
+    <t>УЗ Лайт 2.0</t>
+  </si>
+  <si>
+    <t>LineMech, LineMount</t>
+  </si>
+  <si>
+    <t>Сметно-аналитический комплекс А0</t>
+  </si>
+  <si>
+    <t>Acrobat Pro</t>
+  </si>
+  <si>
+    <t>Creative Cloud — Все приложения</t>
+  </si>
+  <si>
+    <t>Kaspersky Endpoint Security</t>
+  </si>
+  <si>
+    <t>Kaspersky Security для виртуальных и облачных сред, Desktop Russian Edition</t>
+  </si>
+  <si>
+    <t>Kaspersky Security для виртуальных и облачных сред, Server Russian Edition</t>
+  </si>
+  <si>
+    <t>Kaspersky Endpoint Security для бизнеса – Стандартный Russian Edition</t>
+  </si>
+  <si>
+    <t>Kaspersky Endpoint Security for Business - Select Kazakhstan Edition</t>
+  </si>
+  <si>
+    <t>goodhost.kz Хостинг</t>
+  </si>
+  <si>
+    <t>ps.kz Домен</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>AnyDesk</t>
+  </si>
+  <si>
+    <t>FIGMA</t>
+  </si>
+  <si>
+    <t>ДОМЕН irida.company</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Курапов С.В. ; project143)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Щербаков С. Е. ; project106)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Уметбаев Б. Р. ; project135)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 24.0 (Галактионов В. В. ; project141)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 24.0 (Сабиров Р. И. ; project132)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 24.0 (Сабиров А. И. ; project139)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 24.0 (Валиахметов У. Р. ; project120)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 24.0 (Ибатуллин А. И. ; project144)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Гриво Е.А. ; project159)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Чекурдаев К.В. ; project162)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Халиков Р.Р. ; project157)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Усманов Т.Ш. ; project110)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Ахметдинов Д.А. ; project160)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Язев А.В. ; project115)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Савельев И.О. ; project131)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Хасанов Р.Ф. ; project153)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Газизов А.А. ; project117)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 24.0 (Шадров Д.А. ; Project138)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Ямгутдинов Ф. Ф. ; integra09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Хаджиди К.В. ; SVOS24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Гайнетдинов Р.А. ; Project145)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Редников А.А. ; SVOS23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Мангутов А.Ф. ;  SVOS025)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Байгуватов А.С. ; Project147)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Стратичук Н.Н. ; TOKNNOV41)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 23.0 (Еловенкова Е.С. ; project-mini05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD 24.0 (Хасанов А.Ф. ; Project156)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD Металлоконструкции 22.0 x64 (Щербаков С. Е. ; project106)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD Металлоконструкции 22.0 x64 (Уметбаев Б. Р. ; project135)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD BIM Электро 24.0 (Валиахметов У. Р. ; project120)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD BIM Электро 23.0 (Хасанов Р.Ф. ; project153)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NanoCAD BIM Электро 23.0 (Газизов А.А. ; project117)</t>
   </si>
 </sst>
 </file>
@@ -90,22 +207,18 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Hind Vadodara"/>
+      <color rgb="FF3E4676"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -156,19 +269,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,16 +588,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="71.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -494,194 +610,482 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4">
-        <v>45423</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45727</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45528</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="3">
+        <v>45561</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45605</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="3">
+        <v>45612</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="4">
+        <v>45695</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3">
+        <v>45580</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="3">
+        <v>45580</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="3">
+        <v>45565</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3">
+        <v>45598</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="3">
+        <v>45593</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="3">
+        <v>45593</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="3">
+        <v>45593</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="3">
+        <v>45593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="3">
+        <v>45646</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45591</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4">
-        <v>45424</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="B47" s="5">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4">
-        <v>45425</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="B48" s="5">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="5">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4">
-        <v>45426</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4">
-        <v>45427</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4">
-        <v>45428</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4">
-        <v>45429</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="4">
-        <v>45430</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
-        <v>45431</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="4">
-        <v>45432</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4">
-        <v>45433</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4">
-        <v>45434</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4">
-        <v>45435</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4">
-        <v>45436</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4">
-        <v>45437</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="4">
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="4">
-        <v>45439</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4">
-        <v>45440</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="4">
-        <v>45441</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="3" t="s">
+      <c r="B50" s="5">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="4">
-        <v>45442</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="3" t="s">
+      <c r="B51" s="5">
+        <v>45482</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="4">
-        <v>45443</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
+      <c r="B52" s="5">
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="4">
-        <v>45444</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="4">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="4">
-        <v>45446</v>
+      <c r="B53" s="5">
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="5">
+        <v>45657</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="3">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="3">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="3">
+        <v>45597</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="3">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="3">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="3">
+        <v>45794</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="3">
+        <v>45799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>